<commit_message>
Remove typos and wrong naming
</commit_message>
<xml_diff>
--- a/dataAnalysis/tables/monetaryFactors/monetaryFactors.xlsx
+++ b/dataAnalysis/tables/monetaryFactors/monetaryFactors.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5dff752d5d1d42c6/Dokumente/Studium/UniLu/Masterarbeit 2/Masterthesis/dataAnalysis/tables/monetaryFactors/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="267" documentId="11_F25DC773A252ABDACC1048C1511B59885ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{588E3E95-A3A7-4AFF-B7A4-67A42B8331F2}"/>
+  <xr:revisionPtr revIDLastSave="270" documentId="11_F25DC773A252ABDACC1048C1511B59885ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D71C6FA8-D6A3-4376-9E19-303464D81D07}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>team</t>
   </si>
@@ -119,12 +119,6 @@
   </si>
   <si>
     <t>2021/2022</t>
-  </si>
-  <si>
-    <t>2018/2020</t>
-  </si>
-  <si>
-    <t>2018/2021</t>
   </si>
   <si>
     <t>teamBudgetLessBroadcasting_t</t>
@@ -458,8 +452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -487,10 +481,10 @@
         <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F1" t="s">
         <v>16</v>
@@ -549,7 +543,7 @@
         <v>68</v>
       </c>
       <c r="K2" s="1">
-        <f t="shared" ref="K2:K15" si="1">H2/(H2+I2)</f>
+        <f>H2/(H2+I2)</f>
         <v>0.54411764705882348</v>
       </c>
     </row>
@@ -567,7 +561,7 @@
         <v>1450000</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E15" si="2">C3-D3</f>
+        <f t="shared" ref="E3:E15" si="1">C3-D3</f>
         <v>5050000</v>
       </c>
       <c r="F3">
@@ -591,7 +585,7 @@
         <v>56</v>
       </c>
       <c r="K3" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="K2:K15" si="2">H3/(H3+I3)</f>
         <v>0.48214285714285715</v>
       </c>
     </row>
@@ -609,7 +603,7 @@
         <v>1450000</v>
       </c>
       <c r="E4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>9550000</v>
       </c>
       <c r="F4">
@@ -633,7 +627,7 @@
         <v>61</v>
       </c>
       <c r="K4" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.24590163934426229</v>
       </c>
     </row>
@@ -651,7 +645,7 @@
         <v>1450000</v>
       </c>
       <c r="E5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>13550000</v>
       </c>
       <c r="F5">
@@ -675,7 +669,7 @@
         <v>66</v>
       </c>
       <c r="K5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.74242424242424243</v>
       </c>
     </row>
@@ -693,7 +687,7 @@
         <v>1450000</v>
       </c>
       <c r="E6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>13550000</v>
       </c>
       <c r="F6">
@@ -717,7 +711,7 @@
         <v>56</v>
       </c>
       <c r="K6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.4107142857142857</v>
       </c>
     </row>
@@ -759,7 +753,7 @@
         <v>68</v>
       </c>
       <c r="K7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.58823529411764708</v>
       </c>
     </row>
@@ -777,7 +771,7 @@
         <v>1450000</v>
       </c>
       <c r="E8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6850000</v>
       </c>
       <c r="F8">
@@ -801,7 +795,7 @@
         <v>56</v>
       </c>
       <c r="K8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.4642857142857143</v>
       </c>
     </row>
@@ -843,7 +837,7 @@
         <v>61</v>
       </c>
       <c r="K9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.42622950819672129</v>
       </c>
     </row>
@@ -861,7 +855,7 @@
         <v>1450000</v>
       </c>
       <c r="E10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>5650000</v>
       </c>
       <c r="F10">
@@ -885,7 +879,7 @@
         <v>51</v>
       </c>
       <c r="K10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.17647058823529413</v>
       </c>
     </row>
@@ -903,7 +897,7 @@
         <v>1450000</v>
       </c>
       <c r="E11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>12550000</v>
       </c>
       <c r="F11">
@@ -927,7 +921,7 @@
         <v>55</v>
       </c>
       <c r="K11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.45454545454545453</v>
       </c>
     </row>
@@ -936,7 +930,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C12">
         <v>12700000</v>
@@ -945,7 +939,7 @@
         <v>1450000</v>
       </c>
       <c r="E12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>11250000</v>
       </c>
       <c r="F12">
@@ -969,7 +963,7 @@
         <v>55</v>
       </c>
       <c r="K12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.47272727272727272</v>
       </c>
     </row>
@@ -978,7 +972,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C13">
         <v>18400000</v>
@@ -987,7 +981,7 @@
         <v>1450000</v>
       </c>
       <c r="E13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>16950000</v>
       </c>
       <c r="F13">
@@ -1011,7 +1005,7 @@
         <v>55</v>
       </c>
       <c r="K13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.61818181818181817</v>
       </c>
     </row>
@@ -1029,7 +1023,7 @@
         <v>1450000</v>
       </c>
       <c r="E14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>7150000</v>
       </c>
       <c r="F14">
@@ -1053,7 +1047,7 @@
         <v>56</v>
       </c>
       <c r="K14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.375</v>
       </c>
     </row>
@@ -1071,7 +1065,7 @@
         <v>1450000</v>
       </c>
       <c r="E15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>8950000</v>
       </c>
       <c r="F15">
@@ -1095,7 +1089,7 @@
         <v>61</v>
       </c>
       <c r="K15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.37704918032786883</v>
       </c>
     </row>

</xml_diff>